<commit_message>
renamed the vignette files so they appear in desired order
</commit_message>
<xml_diff>
--- a/data/project_optimizedparams.log.xlsx
+++ b/data/project_optimizedparams.log.xlsx
@@ -1257,200 +1257,200 @@
       <c r="E2" t="s">
         <v>139</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-0.1695461</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>-2.4057805</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V2" t="n">
-        <v>1</v>
-      </c>
-      <c r="W2" t="n">
-        <v>1</v>
-      </c>
-      <c r="X2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY2" t="n">
-        <v>-1.6155334</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN2" t="n">
-        <v>1.8240505</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>2.1299459</v>
-      </c>
-      <c r="BP2" t="n">
-        <v>2.0846176</v>
-      </c>
-      <c r="BQ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BR2" t="n">
-        <v>1.6661713</v>
+      <c r="F2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K2" t="s">
+        <v>140</v>
+      </c>
+      <c r="L2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N2" t="s">
+        <v>140</v>
+      </c>
+      <c r="O2" t="s">
+        <v>140</v>
+      </c>
+      <c r="P2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>143</v>
+      </c>
+      <c r="R2" t="s">
+        <v>143</v>
+      </c>
+      <c r="S2" t="s">
+        <v>143</v>
+      </c>
+      <c r="T2" t="s">
+        <v>143</v>
+      </c>
+      <c r="U2" t="s">
+        <v>143</v>
+      </c>
+      <c r="V2" t="s">
+        <v>143</v>
+      </c>
+      <c r="W2" t="s">
+        <v>143</v>
+      </c>
+      <c r="X2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>148</v>
       </c>
       <c r="BS2" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
set vignette index titles to match the rmd document titles.
</commit_message>
<xml_diff>
--- a/data/project_optimizedparams.log.xlsx
+++ b/data/project_optimizedparams.log.xlsx
@@ -1257,200 +1257,200 @@
       <c r="E2" t="s">
         <v>139</v>
       </c>
-      <c r="F2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" t="s">
-        <v>140</v>
-      </c>
-      <c r="I2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J2" t="s">
-        <v>140</v>
-      </c>
-      <c r="K2" t="s">
-        <v>140</v>
-      </c>
-      <c r="L2" t="s">
-        <v>140</v>
-      </c>
-      <c r="M2" t="s">
-        <v>142</v>
-      </c>
-      <c r="N2" t="s">
-        <v>140</v>
-      </c>
-      <c r="O2" t="s">
-        <v>140</v>
-      </c>
-      <c r="P2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>143</v>
-      </c>
-      <c r="R2" t="s">
-        <v>143</v>
-      </c>
-      <c r="S2" t="s">
-        <v>143</v>
-      </c>
-      <c r="T2" t="s">
-        <v>143</v>
-      </c>
-      <c r="U2" t="s">
-        <v>143</v>
-      </c>
-      <c r="V2" t="s">
-        <v>143</v>
-      </c>
-      <c r="W2" t="s">
-        <v>143</v>
-      </c>
-      <c r="X2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>145</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>146</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>147</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>148</v>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-0.1695461</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-2.4057805</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>-1.6155334</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>1.8240505</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>2.1299459</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>2.0846176</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>1.6661713</v>
       </c>
       <c r="BS2" t="s">
         <v>140</v>

</xml_diff>